<commit_message>
get data to db
</commit_message>
<xml_diff>
--- a/CSV/slowka B2.xlsx
+++ b/CSV/slowka B2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dell\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TomeX\IdeaProjects\VerbVault\CSV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1CB794D-8626-4E61-827F-D27E75225946}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4825DAB-F658-4136-A945-2FF2643D151B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -647,10 +647,10 @@
       <selection activeCell="B1" sqref="B1:B50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.33203125" customWidth="1"/>
-    <col min="2" max="2" width="17.6640625" customWidth="1"/>
+    <col min="1" max="1" width="14.28515625" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">

</xml_diff>